<commit_message>
perbaikan daftar mahasiswa alpha
</commit_message>
<xml_diff>
--- a/public/template_absensi.xlsx
+++ b/public/template_absensi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\pbl_kompen\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E259DB7A-179E-4697-A788-6C2E20E14484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EAF858-2D01-4C76-BA3C-C2183126FB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="2070" windowWidth="13290" windowHeight="7110" xr2:uid="{A4983148-5F8B-4A26-AC03-15E6316EC220}"/>
+    <workbookView xWindow="6855" yWindow="1710" windowWidth="13290" windowHeight="7110" xr2:uid="{A4983148-5F8B-4A26-AC03-15E6316EC220}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t>mahasiswa_id</t>
-  </si>
-  <si>
-    <t>sakit</t>
-  </si>
-  <si>
-    <t>izin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>alpha</t>
   </si>
@@ -57,13 +48,16 @@
     <t>periode</t>
   </si>
   <si>
-    <t>kompen</t>
-  </si>
-  <si>
     <t>2024/2025</t>
   </si>
   <si>
-    <t>2024/2026</t>
+    <t>nim</t>
+  </si>
+  <si>
+    <t>Lunas</t>
+  </si>
+  <si>
+    <t>Belum Lunas</t>
   </si>
 </sst>
 </file>
@@ -421,81 +415,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D07F10E-39B6-4DD7-BCDE-045D773F516C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2241760112</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2241760111</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
+      <c r="E3" t="s">
         <v>4</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>